<commit_message>
multi-campaign skeleton, facebookstate, etc.
</commit_message>
<xml_diff>
--- a/adopt/test/example_ads_conf_fly.xlsx
+++ b/adopt/test/example_ads_conf_fly.xlsx
@@ -5,23 +5,24 @@
   <sheets>
     <sheet state="visible" name="user" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="general" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="destination" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="creative" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="targeting" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="targeting_distribution" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="recruitment_experiment" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="destination" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="creative" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="targeting" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="targeting_distribution" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mif4QH5hUtcTjGTVygZMIi1LXxvow=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataSignature="AMtx7mjkUGFb13/ehJme+0mjV1BVFjLF4w=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>key</t>
   </si>
@@ -107,28 +108,31 @@
     <t>US</t>
   </si>
   <si>
+    <t>arms</t>
+  </si>
+  <si>
+    <t>recruitment_days</t>
+  </si>
+  <si>
+    <t>offset_days</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>fly</t>
+  </si>
+  <si>
     <t>initial_shortcode</t>
   </si>
   <si>
     <t>vapingpregate</t>
   </si>
   <si>
-    <t>survey_shortcodes</t>
-  </si>
-  <si>
-    <t>foo, bar</t>
-  </si>
-  <si>
-    <t>finished_question_ref</t>
-  </si>
-  <si>
-    <t>ecigarette_smoke_future</t>
-  </si>
-  <si>
     <t>tags</t>
   </si>
   <si>
-    <t>name</t>
+    <t>destination</t>
   </si>
   <si>
     <t>image_hash</t>
@@ -272,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -305,9 +309,21 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -359,6 +375,10 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -6695,10 +6715,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="23.86"/>
-    <col customWidth="1" min="2" max="2" width="38.57"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="14" t="s">
@@ -6708,35 +6724,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2">
+      <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="16">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="15" t="s">
+      <c r="B3" s="16">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>31</v>
+      <c r="B4" s="16">
+        <v>20.0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" ht="15.0" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -6744,6 +6754,65 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="23.86"/>
+    <col customWidth="1" min="2" max="2" width="38.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" ht="15.0" customHeight="1">
+      <c r="A2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" ht="15.0" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" ht="15.0" customHeight="1">
+      <c r="A4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" ht="15.0" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
@@ -6754,178 +6823,199 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="11.0"/>
-    <col customWidth="1" min="2" max="2" width="27.71"/>
-    <col customWidth="1" min="3" max="3" width="20.43"/>
-    <col customWidth="1" min="4" max="4" width="27.57"/>
-    <col customWidth="1" min="5" max="5" width="30.29"/>
-    <col customWidth="1" min="6" max="6" width="28.43"/>
-    <col customWidth="1" min="7" max="7" width="15.43"/>
-    <col customWidth="1" min="8" max="27" width="8.86"/>
+    <col customWidth="1" min="2" max="2" width="14.43"/>
+    <col customWidth="1" min="3" max="3" width="27.71"/>
+    <col customWidth="1" min="4" max="4" width="20.43"/>
+    <col customWidth="1" min="5" max="5" width="27.57"/>
+    <col customWidth="1" min="6" max="6" width="30.29"/>
+    <col customWidth="1" min="7" max="7" width="28.43"/>
+    <col customWidth="1" min="8" max="8" width="15.43"/>
+    <col customWidth="1" min="9" max="28" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="C1" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="21" t="s">
         <v>40</v>
       </c>
+      <c r="H1" s="21" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
-        <v>41</v>
+      <c r="B2" s="18" t="s">
+        <v>32</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="20" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="23" t="s">
         <v>46</v>
       </c>
+      <c r="H2" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>47</v>
+      <c r="B3" s="18" t="s">
+        <v>32</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>42</v>
+      <c r="C3" s="3" t="s">
+        <v>48</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="20" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="23" t="s">
         <v>46</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="24"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="24"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="12"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" ht="12.0" customHeight="1"/>
     <row r="16" ht="12.0" customHeight="1"/>
@@ -7920,7 +8010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -7943,27 +8033,27 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="7"/>
-      <c r="D3" s="21"/>
+      <c r="D3" s="25"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>
@@ -11950,7 +12040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
@@ -11966,137 +12056,137 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>52</v>
+      <c r="B1" s="28" t="s">
+        <v>53</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
     <row r="2" ht="12.0" customHeight="1">
-      <c r="A2" s="23" t="s">
-        <v>53</v>
+      <c r="A2" s="27" t="s">
+        <v>54</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>54</v>
+      <c r="C2" s="28" t="s">
+        <v>55</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" ht="12.0" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="29">
         <v>0.5</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="29">
         <v>0.5</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" ht="12.0" customHeight="1">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
     </row>
     <row r="8">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
-      <c r="C9" s="26"/>
+      <c r="C9" s="30"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
-      <c r="C10" s="26"/>
+      <c r="C10" s="30"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="C11" s="26"/>
+      <c r="C11" s="30"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
-      <c r="C12" s="26"/>
+      <c r="C12" s="30"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="C13" s="26"/>
+      <c r="C13" s="30"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
-      <c r="C14" s="26"/>
+      <c r="C14" s="30"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
-      <c r="C15" s="26"/>
+      <c r="C15" s="30"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
-      <c r="C16" s="26"/>
+      <c r="C16" s="30"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
-      <c r="C17" s="26"/>
+      <c r="C17" s="30"/>
     </row>
     <row r="18" ht="12.0" customHeight="1"/>
     <row r="19" ht="12.0" customHeight="1"/>

</xml_diff>

<commit_message>
recruitment experiments, end dates
</commit_message>
<xml_diff>
--- a/adopt/test/example_ads_conf_fly.xlsx
+++ b/adopt/test/example_ads_conf_fly.xlsx
@@ -5,24 +5,26 @@
   <sheets>
     <sheet state="visible" name="user" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="general" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="recruitment_experiment" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="destination" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="creative" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="targeting" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="targeting_distribution" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="recruitment_simple" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="recruitment_destination_experim" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="recruitment_pipeline_experiment" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="destination" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="creative" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="targeting" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="targeting_distribution" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataSignature="AMtx7mjkUGFb13/ehJme+0mjV1BVFjLF4w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mgOMmeAUQMXqjmWJs2i5dSwfgIs7w=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>key</t>
   </si>
@@ -34,6 +36,12 @@
   </si>
   <si>
     <t>nandanmarkrao@gmail.com</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>example-fly-conf</t>
   </si>
   <si>
     <t>optimization_goal</t>
@@ -60,9 +68,6 @@
     <t>48</t>
   </si>
   <si>
-    <t>proportional</t>
-  </si>
-  <si>
     <t>page_id</t>
   </si>
   <si>
@@ -81,6 +86,18 @@
     <t>1342820622846299</t>
   </si>
   <si>
+    <t>extra_metadata</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>country_code</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
     <t>ad_campaign_name</t>
   </si>
   <si>
@@ -96,16 +113,16 @@
     <t>end_date</t>
   </si>
   <si>
-    <t>extra_metadata</t>
+    <t>ad_campaign_name_base</t>
   </si>
   <si>
-    <t>{}</t>
+    <t>budget_per_arm</t>
   </si>
   <si>
-    <t>country_code</t>
+    <t>destinations</t>
   </si>
   <si>
-    <t>US</t>
+    <t>lottery, topup</t>
   </si>
   <si>
     <t>arms</t>
@@ -115,9 +132,6 @@
   </si>
   <si>
     <t>offset_days</t>
-  </si>
-  <si>
-    <t>name</t>
   </si>
   <si>
     <t>fly</t>
@@ -276,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -287,19 +301,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -312,6 +326,30 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -319,14 +357,8 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -379,6 +411,14 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -638,202 +678,186 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="5"/>
     </row>
     <row r="3" ht="15.0" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="5"/>
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="B7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="5"/>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" ht="15.0" customHeight="1">
-      <c r="A9" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" ht="15.0" customHeight="1">
+      <c r="A9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="5"/>
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" ht="15.0" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4">
-        <v>8400.0</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" ht="15.0" customHeight="1">
-      <c r="A12" s="3" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" ht="15.0" customHeight="1">
+      <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="10">
-        <v>44571.0</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" ht="15.0" customHeight="1">
-      <c r="A13" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="10">
-        <v>44592.0</v>
-      </c>
-      <c r="C13" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" ht="15.0" customHeight="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" ht="15.0" customHeight="1">
+      <c r="A13" s="3"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14" ht="15.0" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" ht="15.0" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" ht="15.0" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" ht="15.0" customHeight="1">
+    <row r="15" ht="15.0" customHeight="1"/>
+    <row r="16" ht="15.0" customHeight="1"/>
+    <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" ht="15.0" customHeight="1">
-      <c r="C18" s="7"/>
+    <row r="18" ht="12.0" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" ht="15.0" customHeight="1"/>
-    <row r="20" ht="15.0" customHeight="1"/>
+    <row r="19" ht="12.0" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" ht="12.0" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="5"/>
+    </row>
     <row r="21" ht="12.0" customHeight="1">
-      <c r="A21" s="3"/>
+      <c r="A21" s="5"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="7"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="5"/>
     </row>
     <row r="22" ht="12.0" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="7"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="5"/>
     </row>
     <row r="23" ht="12.0" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="13"/>
       <c r="D23" s="5"/>
     </row>
     <row r="24" ht="12.0" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="13"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
     <row r="25" ht="12.0" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="13"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="5"/>
     </row>
     <row r="26" ht="12.0" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="13"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
     <row r="27" ht="12.0" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="5"/>
     </row>
     <row r="28" ht="12.0" customHeight="1">
@@ -6673,30 +6697,6 @@
       <c r="B1000" s="4"/>
       <c r="C1000" s="5"/>
       <c r="D1000" s="5"/>
-    </row>
-    <row r="1001" ht="12.0" customHeight="1">
-      <c r="A1001" s="5"/>
-      <c r="B1001" s="4"/>
-      <c r="C1001" s="5"/>
-      <c r="D1001" s="5"/>
-    </row>
-    <row r="1002" ht="12.0" customHeight="1">
-      <c r="A1002" s="5"/>
-      <c r="B1002" s="4"/>
-      <c r="C1002" s="5"/>
-      <c r="D1002" s="5"/>
-    </row>
-    <row r="1003" ht="12.0" customHeight="1">
-      <c r="A1003" s="5"/>
-      <c r="B1003" s="4"/>
-      <c r="C1003" s="5"/>
-      <c r="D1003" s="5"/>
-    </row>
-    <row r="1004" ht="12.0" customHeight="1">
-      <c r="A1004" s="5"/>
-      <c r="B1004" s="4"/>
-      <c r="C1004" s="5"/>
-      <c r="D1004" s="5"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -6715,6 +6715,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="22.29"/>
+    <col customWidth="1" min="2" max="2" width="21.29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="14" t="s">
@@ -6725,27 +6729,35 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="4">
+        <v>8400.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="16">
+        <v>44571.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="16">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="16">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="16">
-        <v>20.0</v>
+      <c r="B5" s="16">
+        <v>44592.0</v>
       </c>
     </row>
   </sheetData>
@@ -6763,49 +6775,57 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.86"/>
-    <col customWidth="1" min="2" max="2" width="38.57"/>
+    <col customWidth="1" min="1" max="1" width="26.86"/>
+    <col customWidth="1" min="2" max="2" width="31.43"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="18" t="s">
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4">
+        <v>8400.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="16">
+        <v>44571.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="16">
+        <v>44592.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" ht="15.0" customHeight="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" ht="15.0" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -6813,6 +6833,144 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="25.29"/>
+    <col customWidth="1" min="2" max="2" width="29.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4">
+        <v>8400.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="16">
+        <v>44571.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="20">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="22">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="22">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="23.86"/>
+    <col customWidth="1" min="2" max="2" width="38.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" ht="15.0" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" ht="15.0" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" ht="15.0" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" ht="15.0" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="5"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
@@ -6834,107 +6992,107 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="21" t="s">
-        <v>35</v>
+      <c r="A1" s="27" t="s">
+        <v>39</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" ht="12.0" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>31</v>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" ht="12.0" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>43</v>
+      <c r="D2" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>46</v>
+      <c r="G2" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" ht="12.0" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" ht="12.0" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>43</v>
+      <c r="F3" s="3" t="s">
+        <v>49</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>46</v>
+      <c r="G3" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="24"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="23"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="24"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="23"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="24"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="23"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
@@ -6944,7 +7102,7 @@
       <c r="D7" s="12"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="23"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
@@ -6954,7 +7112,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="23"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
@@ -6964,7 +7122,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="23"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
@@ -6974,7 +7132,7 @@
       <c r="D10" s="12"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
@@ -6984,7 +7142,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="23"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
@@ -6994,7 +7152,7 @@
       <c r="D12" s="12"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="23"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
@@ -7004,7 +7162,7 @@
       <c r="D13" s="12"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="23"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
@@ -7014,7 +7172,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" ht="12.0" customHeight="1"/>
@@ -8010,7 +8168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -8033,27 +8191,27 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="25"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="C4" s="7"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>
@@ -12040,7 +12198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
@@ -12056,137 +12214,137 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="27" t="s">
-        <v>52</v>
+      <c r="A1" s="33" t="s">
+        <v>56</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>53</v>
+      <c r="B1" s="34" t="s">
+        <v>57</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>53</v>
+      <c r="C1" s="34" t="s">
+        <v>57</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
     <row r="2" ht="12.0" customHeight="1">
-      <c r="A2" s="27" t="s">
-        <v>54</v>
+      <c r="A2" s="33" t="s">
+        <v>58</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>9</v>
+      <c r="B2" s="34" t="s">
+        <v>11</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>55</v>
+      <c r="C2" s="34" t="s">
+        <v>59</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" ht="12.0" customHeight="1">
-      <c r="A3" s="29" t="s">
-        <v>27</v>
+      <c r="A3" s="35" t="s">
+        <v>23</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="35">
         <v>0.5</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="35">
         <v>0.5</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
     </row>
     <row r="4" ht="12.0" customHeight="1">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
     </row>
     <row r="8">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
-      <c r="C9" s="30"/>
+      <c r="C9" s="36"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
-      <c r="C10" s="30"/>
+      <c r="C10" s="36"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="C11" s="30"/>
+      <c r="C11" s="36"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
-      <c r="C12" s="30"/>
+      <c r="C12" s="36"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="C13" s="30"/>
+      <c r="C13" s="36"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
-      <c r="C14" s="30"/>
+      <c r="C14" s="36"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
-      <c r="C15" s="30"/>
+      <c r="C15" s="36"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
-      <c r="C16" s="30"/>
+      <c r="C16" s="36"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
-      <c r="C17" s="30"/>
+      <c r="C17" s="36"/>
     </row>
     <row r="18" ht="12.0" customHeight="1"/>
     <row r="19" ht="12.0" customHeight="1"/>

</xml_diff>

<commit_message>
added max_sample to recruitment conf and optimization
</commit_message>
<xml_diff>
--- a/adopt/test/example_ads_conf_fly.xlsx
+++ b/adopt/test/example_ads_conf_fly.xlsx
@@ -17,14 +17,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mgOMmeAUQMXqjmWJs2i5dSwfgIs7w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mjqgbHsZQsG/qaq29lgDbCPKuKuPA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
   <si>
     <t>key</t>
   </si>
@@ -107,6 +107,9 @@
     <t>budget</t>
   </si>
   <si>
+    <t>max_sample</t>
+  </si>
+  <si>
     <t>start_date</t>
   </si>
   <si>
@@ -117,6 +120,9 @@
   </si>
   <si>
     <t>budget_per_arm</t>
+  </si>
+  <si>
+    <t>max_sample_per_arm</t>
   </si>
   <si>
     <t>destinations</t>
@@ -290,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -328,6 +334,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
@@ -6745,18 +6754,26 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="16">
-        <v>44571.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="17">
+        <v>44571.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="17">
         <v>44592.0</v>
       </c>
     </row>
@@ -6789,7 +6806,7 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>25</v>
@@ -6797,34 +6814,42 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4">
         <v>8400.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
+      <c r="A4" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B4" s="16">
-        <v>44571.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="17">
+        <v>44571.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="17">
         <v>44592.0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="17" t="s">
-        <v>31</v>
+    <row r="7">
+      <c r="A7" s="18" t="s">
+        <v>33</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>32</v>
+      <c r="B7" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -6856,7 +6881,7 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>25</v>
@@ -6864,47 +6889,55 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4">
         <v>8400.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
+      <c r="A4" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B4" s="16">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="17">
         <v>44571.0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="19" t="s">
-        <v>33</v>
+    <row r="6">
+      <c r="A6" s="20" t="s">
+        <v>35</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B6" s="21">
         <v>2.0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="21" t="s">
-        <v>34</v>
+    <row r="7">
+      <c r="A7" s="22" t="s">
+        <v>36</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B7" s="23">
         <v>10.0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="21" t="s">
-        <v>35</v>
+    <row r="8">
+      <c r="A8" s="22" t="s">
+        <v>37</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B8" s="23">
         <v>20.0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
+    <row r="9">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -6926,10 +6959,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6937,25 +6970,25 @@
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>36</v>
+      <c r="B2" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="5"/>
     </row>
     <row r="3" ht="15.0" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="18"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="8"/>
       <c r="D4" s="5"/>
     </row>
@@ -6992,107 +7025,107 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="27" t="s">
-        <v>39</v>
+      <c r="A1" s="28" t="s">
+        <v>41</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>40</v>
+      <c r="B1" s="29" t="s">
+        <v>42</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="28" t="s">
+      <c r="D1" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="E1" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="F1" s="29" t="s">
         <v>45</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>47</v>
+      <c r="D2" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>50</v>
+      <c r="G2" s="30" t="s">
+        <v>52</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>50</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="30"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="29"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="30"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="29"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="30"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="29"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
@@ -7102,7 +7135,7 @@
       <c r="D7" s="12"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="29"/>
+      <c r="G7" s="30"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
@@ -7112,7 +7145,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="29"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
@@ -7122,7 +7155,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="29"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
@@ -7132,7 +7165,7 @@
       <c r="D10" s="12"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="29"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
@@ -7142,7 +7175,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="29"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
@@ -7152,7 +7185,7 @@
       <c r="D12" s="12"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="29"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
@@ -7162,7 +7195,7 @@
       <c r="D13" s="12"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="29"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
@@ -7172,7 +7205,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="29"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" ht="12.0" customHeight="1"/>
@@ -8191,27 +8224,27 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="31"/>
+      <c r="D3" s="32"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="C4" s="8"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>
@@ -12214,137 +12247,137 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="33" t="s">
-        <v>56</v>
+      <c r="A1" s="34" t="s">
+        <v>58</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>57</v>
+      <c r="B1" s="35" t="s">
+        <v>59</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>57</v>
+      <c r="C1" s="35" t="s">
+        <v>59</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
     <row r="2" ht="12.0" customHeight="1">
-      <c r="A2" s="33" t="s">
-        <v>58</v>
+      <c r="A2" s="34" t="s">
+        <v>60</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>59</v>
+      <c r="C2" s="35" t="s">
+        <v>61</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" ht="12.0" customHeight="1">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="36">
         <v>0.5</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="36">
         <v>0.5</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
     </row>
     <row r="4" ht="12.0" customHeight="1">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
     </row>
     <row r="8">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
-      <c r="C9" s="36"/>
+      <c r="C9" s="37"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
-      <c r="C10" s="36"/>
+      <c r="C10" s="37"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="C11" s="36"/>
+      <c r="C11" s="37"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
-      <c r="C12" s="36"/>
+      <c r="C12" s="37"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="C13" s="36"/>
+      <c r="C13" s="37"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
-      <c r="C14" s="36"/>
+      <c r="C14" s="37"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
-      <c r="C15" s="36"/>
+      <c r="C15" s="37"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
-      <c r="C16" s="36"/>
+      <c r="C16" s="37"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
-      <c r="C17" s="36"/>
+      <c r="C17" s="37"/>
     </row>
     <row r="18" ht="12.0" customHeight="1"/>
     <row r="19" ht="12.0" customHeight="1"/>

</xml_diff>

<commit_message>
using one db connection across tests to avoid race conditions
</commit_message>
<xml_diff>
--- a/adopt/test/example_ads_conf_fly.xlsx
+++ b/adopt/test/example_ads_conf_fly.xlsx
@@ -17,14 +17,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mjqgbHsZQsG/qaq29lgDbCPKuKuPA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mi/cB25FKfVnkZfKoHUs4++7aBPNg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
   <si>
     <t>key</t>
   </si>
@@ -219,11 +219,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -252,6 +253,11 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -259,6 +265,11 @@
       <b/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -296,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -319,20 +330,20 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -344,8 +355,14 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -359,15 +376,18 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -375,18 +395,18 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -6913,31 +6933,39 @@
     </row>
     <row r="6">
       <c r="A6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="21">
+        <v>44601.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B7" s="23">
         <v>2.0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="22" t="s">
+    <row r="8">
+      <c r="A8" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B8" s="25">
         <v>10.0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="22" t="s">
+    <row r="9">
+      <c r="A9" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B9" s="25">
         <v>20.0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
+    <row r="10">
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -6959,10 +6987,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6970,7 +6998,7 @@
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="8"/>
@@ -6988,7 +7016,7 @@
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="19"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="8"/>
       <c r="D4" s="5"/>
     </row>
@@ -7025,28 +7053,28 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="31" t="s">
         <v>47</v>
       </c>
     </row>
@@ -7067,7 +7095,7 @@
       <c r="F2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="33" t="s">
         <v>52</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -7091,7 +7119,7 @@
       <c r="F3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="33" t="s">
         <v>52</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -7102,30 +7130,30 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="31"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="30"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="31"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="30"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="31"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="30"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
@@ -7135,7 +7163,7 @@
       <c r="D7" s="12"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="30"/>
+      <c r="G7" s="33"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
@@ -7145,7 +7173,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="30"/>
+      <c r="G8" s="33"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
@@ -7155,7 +7183,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="30"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
@@ -7165,7 +7193,7 @@
       <c r="D10" s="12"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="30"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
@@ -7175,7 +7203,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="30"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
@@ -7185,7 +7213,7 @@
       <c r="D12" s="12"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="30"/>
+      <c r="G12" s="33"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
@@ -7195,7 +7223,7 @@
       <c r="D13" s="12"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="30"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
@@ -7205,7 +7233,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="30"/>
+      <c r="G14" s="33"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" ht="12.0" customHeight="1"/>
@@ -8236,15 +8264,15 @@
         <v>57</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="32"/>
+      <c r="D3" s="35"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="C4" s="8"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>
@@ -12247,137 +12275,137 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
     <row r="2" ht="12.0" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" ht="12.0" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="39">
         <v>0.5</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="39">
         <v>0.5</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" ht="12.0" customHeight="1">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
     </row>
     <row r="8">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
-      <c r="C9" s="37"/>
+      <c r="C9" s="40"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
-      <c r="C10" s="37"/>
+      <c r="C10" s="40"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="C11" s="37"/>
+      <c r="C11" s="40"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
-      <c r="C12" s="37"/>
+      <c r="C12" s="40"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="C13" s="37"/>
+      <c r="C13" s="40"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
-      <c r="C14" s="37"/>
+      <c r="C14" s="40"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
-      <c r="C15" s="37"/>
+      <c r="C15" s="40"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
-      <c r="C16" s="37"/>
+      <c r="C16" s="40"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
-      <c r="C17" s="37"/>
+      <c r="C17" s="40"/>
     </row>
     <row r="18" ht="12.0" customHeight="1"/>
     <row r="19" ht="12.0" customHeight="1"/>

</xml_diff>

<commit_message>
added objective to GeneralConf
</commit_message>
<xml_diff>
--- a/adopt/test/example_ads_conf_fly.xlsx
+++ b/adopt/test/example_ads_conf_fly.xlsx
@@ -17,14 +17,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mi/cB25FKfVnkZfKoHUs4++7aBPNg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mgnZ0yWvgg2zOCicHP7JTDhFM9bEA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>key</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>example-fly-conf</t>
+  </si>
+  <si>
+    <t>objective</t>
+  </si>
+  <si>
+    <t>MESSAGES</t>
   </si>
   <si>
     <t>optimization_goal</t>
@@ -717,10 +723,10 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="8"/>
@@ -777,38 +783,42 @@
       <c r="D8" s="5"/>
     </row>
     <row r="9" ht="15.0" customHeight="1">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="5"/>
     </row>
     <row r="10" ht="15.0" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="5"/>
     </row>
     <row r="11" ht="15.0" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="5"/>
     </row>
     <row r="12" ht="15.0" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="8"/>
       <c r="D12" s="5"/>
     </row>
@@ -819,19 +829,19 @@
       <c r="D13" s="5"/>
     </row>
     <row r="14" ht="15.0" customHeight="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="8"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" ht="15.0" customHeight="1"/>
+    <row r="15" ht="15.0" customHeight="1">
+      <c r="C15" s="8"/>
+      <c r="D15" s="5"/>
+    </row>
     <row r="16" ht="15.0" customHeight="1"/>
-    <row r="17" ht="12.0" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="5"/>
-    </row>
+    <row r="17" ht="15.0" customHeight="1"/>
     <row r="18" ht="12.0" customHeight="1">
-      <c r="A18" s="5"/>
+      <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="5"/>
@@ -839,7 +849,7 @@
     <row r="19" ht="12.0" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="13"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="5"/>
     </row>
     <row r="20" ht="12.0" customHeight="1">
@@ -863,12 +873,12 @@
     <row r="23" ht="12.0" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="4"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="5"/>
     </row>
     <row r="24" ht="12.0" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
     <row r="25" ht="12.0" customHeight="1">
@@ -6726,6 +6736,12 @@
       <c r="B1000" s="4"/>
       <c r="C1000" s="5"/>
       <c r="D1000" s="5"/>
+    </row>
+    <row r="1001" ht="12.0" customHeight="1">
+      <c r="A1001" s="5"/>
+      <c r="B1001" s="4"/>
+      <c r="C1001" s="5"/>
+      <c r="D1001" s="5"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -6759,15 +6775,15 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4">
         <v>8400.0</v>
@@ -6775,7 +6791,7 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" s="16">
         <v>1000.0</v>
@@ -6783,7 +6799,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="17">
         <v>44571.0</v>
@@ -6791,7 +6807,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B6" s="17">
         <v>44592.0</v>
@@ -6826,15 +6842,15 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4">
         <v>8400.0</v>
@@ -6842,7 +6858,7 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="16">
         <v>1000.0</v>
@@ -6850,7 +6866,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="17">
         <v>44571.0</v>
@@ -6858,7 +6874,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B6" s="17">
         <v>44592.0</v>
@@ -6866,10 +6882,10 @@
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -6901,15 +6917,15 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4">
         <v>8400.0</v>
@@ -6917,7 +6933,7 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="16">
         <v>1000.0</v>
@@ -6925,7 +6941,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="17">
         <v>44571.0</v>
@@ -6933,7 +6949,7 @@
     </row>
     <row r="6">
       <c r="A6" s="20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B6" s="21">
         <v>44601.0</v>
@@ -6941,7 +6957,7 @@
     </row>
     <row r="7">
       <c r="A7" s="22" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" s="23">
         <v>2.0</v>
@@ -6949,7 +6965,7 @@
     </row>
     <row r="8">
       <c r="A8" s="24" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B8" s="25">
         <v>10.0</v>
@@ -6957,7 +6973,7 @@
     </row>
     <row r="9">
       <c r="A9" s="24" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B9" s="25">
         <v>20.0</v>
@@ -6999,17 +7015,17 @@
         <v>4</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="5"/>
     </row>
     <row r="3" ht="15.0" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="5"/>
@@ -7054,76 +7070,76 @@
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>52</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" ht="12.0" customHeight="1">
@@ -8252,16 +8268,16 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="35"/>
@@ -12276,13 +12292,13 @@
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
       <c r="A1" s="37" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D1" s="38"/>
       <c r="E1" s="38"/>
@@ -12293,13 +12309,13 @@
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="37" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D2" s="38"/>
       <c r="E2" s="38"/>
@@ -12310,7 +12326,7 @@
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="39" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" s="39">
         <v>0.5</v>

</xml_diff>

<commit_message>
reworked target_distribution format to allow fewer vars
</commit_message>
<xml_diff>
--- a/adopt/test/example_ads_conf_fly.xlsx
+++ b/adopt/test/example_ads_conf_fly.xlsx
@@ -17,14 +17,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mgnZ0yWvgg2zOCicHP7JTDhFM9bEA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mjMF2iQnB6HRTr+VXB+Yqtd3RyIcg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>key</t>
   </si>
@@ -203,7 +203,7 @@
     <t>distribution_vars</t>
   </si>
   <si>
-    <t>gender, age</t>
+    <t>location, gender, age</t>
   </si>
   <si>
     <t>age</t>
@@ -217,6 +217,9 @@
   <si>
     <t>2</t>
   </si>
+  <si>
+    <t>location</t>
+  </si>
 </sst>
 </file>
 
@@ -225,7 +228,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -292,6 +295,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -313,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -411,6 +419,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -8256,6 +8267,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="27.29"/>
+    <col customWidth="1" min="2" max="2" width="20.86"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -8276,7 +8288,7 @@
       <c r="A3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="8"/>
@@ -12326,104 +12338,116 @@
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+    </row>
+    <row r="4" ht="12.0" customHeight="1">
+      <c r="A4" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B4" s="40">
         <v>0.5</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C4" s="40">
         <v>0.5</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-    </row>
-    <row r="4" ht="12.0" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-    </row>
-    <row r="9" ht="12.0" customHeight="1">
-      <c r="C9" s="40"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+    </row>
+    <row r="8" ht="12.0" customHeight="1">
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
-      <c r="C10" s="40"/>
+      <c r="C10" s="41"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="C11" s="40"/>
+      <c r="C11" s="41"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
-      <c r="C12" s="40"/>
+      <c r="C12" s="41"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="C13" s="40"/>
+      <c r="C13" s="41"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
-      <c r="C14" s="40"/>
+      <c r="C14" s="41"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
-      <c r="C15" s="40"/>
+      <c r="C15" s="41"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
-      <c r="C16" s="40"/>
+      <c r="C16" s="41"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
-      <c r="C17" s="40"/>
-    </row>
-    <row r="18" ht="12.0" customHeight="1"/>
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" ht="12.0" customHeight="1">
+      <c r="C18" s="41"/>
+    </row>
     <row r="19" ht="12.0" customHeight="1"/>
     <row r="20" ht="12.0" customHeight="1"/>
     <row r="21" ht="12.0" customHeight="1"/>
@@ -13390,6 +13414,7 @@
     <row r="982" ht="12.0" customHeight="1"/>
     <row r="983" ht="12.0" customHeight="1"/>
     <row r="984" ht="12.0" customHeight="1"/>
+    <row r="985" ht="12.0" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
adopt: removed country_code from GeneralConf
</commit_message>
<xml_diff>
--- a/adopt/test/example_ads_conf_fly.xlsx
+++ b/adopt/test/example_ads_conf_fly.xlsx
@@ -17,14 +17,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mjMF2iQnB6HRTr+VXB+Yqtd3RyIcg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mhytcccxm4hOYis4spHzz1B/hbO0g=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
   <si>
     <t>key</t>
   </si>
@@ -44,10 +44,16 @@
     <t>example-fly-conf</t>
   </si>
   <si>
+    <t>Text field</t>
+  </si>
+  <si>
     <t>objective</t>
   </si>
   <si>
     <t>MESSAGES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select </t>
   </si>
   <si>
     <t>optimization_goal</t>
@@ -74,10 +80,16 @@
     <t>48</t>
   </si>
   <si>
+    <t>Text field?</t>
+  </si>
+  <si>
     <t>page_id</t>
   </si>
   <si>
     <t>1855355231229529</t>
+  </si>
+  <si>
+    <t>Text field for now</t>
   </si>
   <si>
     <t>instagram_id</t>
@@ -98,16 +110,16 @@
     <t>{}</t>
   </si>
   <si>
-    <t>country_code</t>
-  </si>
-  <si>
-    <t>US</t>
+    <t>Check with Nandan</t>
   </si>
   <si>
     <t>ad_campaign_name</t>
   </si>
   <si>
     <t>vlab-vaping-pilot-2</t>
+  </si>
+  <si>
+    <t>Text</t>
   </si>
   <si>
     <t>budget</t>
@@ -119,10 +131,16 @@
     <t>start_date</t>
   </si>
   <si>
+    <t>Text with some inbuilt formatting or calendar dropdown - explore options here</t>
+  </si>
+  <si>
     <t>end_date</t>
   </si>
   <si>
     <t>ad_campaign_name_base</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
   <si>
     <t>budget_per_arm</t>
@@ -135,6 +153,9 @@
   </si>
   <si>
     <t>lottery, topup</t>
+  </si>
+  <si>
+    <t>select</t>
   </si>
   <si>
     <t>arms</t>
@@ -206,6 +227,9 @@
     <t>location, gender, age</t>
   </si>
   <si>
+    <t>multi-select?</t>
+  </si>
+  <si>
     <t>age</t>
   </si>
   <si>
@@ -219,6 +243,9 @@
   </si>
   <si>
     <t>location</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
@@ -321,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -339,16 +366,19 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -360,6 +390,9 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -367,9 +400,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -417,13 +447,19 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -730,123 +766,139 @@
       <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="D2" s="5"/>
     </row>
     <row r="3" ht="15.0" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="D3" s="5"/>
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="8"/>
+        <v>17</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" ht="15.0" customHeight="1">
-      <c r="A10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="8"/>
       <c r="D10" s="5"/>
     </row>
     <row r="11" ht="15.0" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12" ht="15.0" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="8"/>
       <c r="D12" s="5"/>
     </row>
     <row r="13" ht="15.0" customHeight="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="5"/>
     </row>
     <row r="14" ht="15.0" customHeight="1">
       <c r="A14" s="3"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="5"/>
     </row>
     <row r="15" ht="15.0" customHeight="1">
-      <c r="C15" s="8"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="5"/>
     </row>
     <row r="16" ht="15.0" customHeight="1"/>
@@ -854,37 +906,37 @@
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="8"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="5"/>
     </row>
     <row r="19" ht="12.0" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="5"/>
     </row>
     <row r="20" ht="12.0" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="13"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="5"/>
     </row>
     <row r="21" ht="12.0" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="13"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="5"/>
     </row>
     <row r="22" ht="12.0" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="13"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="5"/>
     </row>
     <row r="23" ht="12.0" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="13"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="5"/>
     </row>
     <row r="24" ht="12.0" customHeight="1">
@@ -6777,51 +6829,66 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4">
         <v>8400.0</v>
       </c>
+      <c r="C3" s="17" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="16">
+        <v>33</v>
+      </c>
+      <c r="B4" s="18">
         <v>1000.0</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="17">
+        <v>34</v>
+      </c>
+      <c r="B5" s="19">
         <v>44571.0</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="17">
+        <v>36</v>
+      </c>
+      <c r="B6" s="19">
         <v>44592.0</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -6844,59 +6911,77 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4">
         <v>8400.0</v>
       </c>
+      <c r="C3" s="17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="16">
+        <v>40</v>
+      </c>
+      <c r="B4" s="18">
         <v>1000.0</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="17">
+        <v>34</v>
+      </c>
+      <c r="B5" s="19">
         <v>44571.0</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="17">
+        <v>36</v>
+      </c>
+      <c r="B6" s="19">
         <v>44592.0</v>
       </c>
+      <c r="C6" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>36</v>
+      <c r="A7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -6919,80 +7004,104 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4">
         <v>8400.0</v>
       </c>
+      <c r="C3" s="17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="16">
+        <v>40</v>
+      </c>
+      <c r="B4" s="18">
         <v>1000.0</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="17">
+        <v>34</v>
+      </c>
+      <c r="B5" s="19">
         <v>44571.0</v>
       </c>
+      <c r="C5" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="21">
+      <c r="A6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="22">
         <v>44601.0</v>
       </c>
+      <c r="C6" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="23">
+      <c r="A7" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="24">
         <v>2.0</v>
       </c>
+      <c r="C7" s="17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="26">
+        <v>10.0</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="25">
-        <v>10.0</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="25">
+      <c r="A9" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="26">
         <v>20.0</v>
       </c>
+      <c r="C9" s="17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -7014,10 +7123,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7025,32 +7134,36 @@
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="8"/>
+      <c r="B2" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="D2" s="5"/>
     </row>
     <row r="3" ht="15.0" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="8"/>
+        <v>48</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="D3" s="5"/>
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="5"/>
     </row>
   </sheetData>
@@ -7080,187 +7193,187 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="31" t="s">
+      <c r="A1" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>49</v>
+      <c r="D1" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>54</v>
+        <v>60</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>61</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="6" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>51</v>
+        <v>63</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>54</v>
+        <v>60</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>61</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="34"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="33"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="34"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="33"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="34"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="33"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="12"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="33"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="33"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="12"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="33"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="33"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="33"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="33"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="33"/>
+      <c r="G14" s="34"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" ht="12.0" customHeight="1"/>
@@ -8280,27 +8393,32 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B2" s="5"/>
+      <c r="C2" s="17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="35"/>
+        <v>65</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="C4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>
@@ -12303,150 +12421,150 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="A1" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
     <row r="2" ht="12.0" customHeight="1">
-      <c r="A2" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="A2" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" ht="12.0" customHeight="1">
-      <c r="A3" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
+      <c r="A3" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
     </row>
     <row r="4" ht="12.0" customHeight="1">
-      <c r="A4" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="40">
+      <c r="A4" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="42">
         <v>0.5</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="42">
         <v>0.5</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
     </row>
     <row r="9">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
-      <c r="C10" s="41"/>
+      <c r="C10" s="43"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="C11" s="41"/>
+      <c r="C11" s="43"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
-      <c r="C12" s="41"/>
+      <c r="C12" s="43"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="C13" s="41"/>
+      <c r="C13" s="43"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
-      <c r="C14" s="41"/>
+      <c r="C14" s="43"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
-      <c r="C15" s="41"/>
+      <c r="C15" s="43"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
-      <c r="C16" s="41"/>
+      <c r="C16" s="43"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
-      <c r="C17" s="41"/>
+      <c r="C17" s="43"/>
     </row>
     <row r="18" ht="12.0" customHeight="1">
-      <c r="C18" s="41"/>
+      <c r="C18" s="43"/>
     </row>
     <row r="19" ht="12.0" customHeight="1"/>
     <row r="20" ht="12.0" customHeight="1"/>

</xml_diff>